<commit_message>
plot + failed fx attempt + test file
</commit_message>
<xml_diff>
--- a/SLT practical coordinates.xlsx
+++ b/SLT practical coordinates.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tud365-my.sharepoint.com/personal/mgerits_tudelft_nl/Documents/Documenten/Academia/Study material/Bsc 2/AE2130-II Wind tunnel practical/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tud365-my.sharepoint.com/personal/mgerits_tudelft_nl/Documents/Documenten/Academia/Study material/Bsc 2/AE2130-II Wind tunnel practical/wakeDragCalc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="25" documentId="8_{307C2FEA-5DCC-4CA3-A21B-AE35B7660964}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5D26DF9B-79CB-413D-8421-07603A7E434C}"/>
+  <xr:revisionPtr revIDLastSave="26" documentId="8_{307C2FEA-5DCC-4CA3-A21B-AE35B7660964}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E3ACF625-E688-4BF3-AB50-380B0EE9DDF9}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="24892" windowHeight="14914" xr2:uid="{5EF1D621-4C1B-428B-ABAC-2FCB482E083B}"/>
   </bookViews>
@@ -628,18 +628,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -675,6 +663,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1026,37 +1026,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="1" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="21" t="s">
         <v>119</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="23" t="s">
         <v>116</v>
       </c>
-      <c r="C1" s="12"/>
+      <c r="C1" s="24"/>
       <c r="D1" s="6"/>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="21" t="s">
         <v>117</v>
       </c>
       <c r="G1" s="6"/>
-      <c r="H1" s="9" t="s">
+      <c r="H1" s="21" t="s">
         <v>119</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="I1" s="21" t="s">
         <v>118</v>
       </c>
       <c r="J1" s="6"/>
-      <c r="K1" s="9" t="s">
+      <c r="K1" s="21" t="s">
         <v>119</v>
       </c>
-      <c r="L1" s="9" t="s">
+      <c r="L1" s="21" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="2" spans="1:13" s="1" customFormat="1" ht="15.9" x14ac:dyDescent="0.4">
-      <c r="A2" s="10"/>
+      <c r="A2" s="22"/>
       <c r="B2" s="7" t="s">
         <v>49</v>
       </c>
@@ -1064,14 +1064,14 @@
         <v>50</v>
       </c>
       <c r="D2" s="6"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
       <c r="G2" s="6"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
+      <c r="H2" s="22"/>
+      <c r="I2" s="22"/>
       <c r="J2" s="6"/>
-      <c r="K2" s="10"/>
-      <c r="L2" s="10"/>
+      <c r="K2" s="22"/>
+      <c r="L2" s="22"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A3" s="3" t="s">
@@ -1087,14 +1087,14 @@
       <c r="E3" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="F3" s="13">
+      <c r="F3" s="9">
         <v>0</v>
       </c>
       <c r="G3" s="2"/>
       <c r="H3" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="I3" s="13">
+      <c r="I3" s="9">
         <v>43.5</v>
       </c>
       <c r="J3" s="2"/>
@@ -1120,14 +1120,14 @@
       <c r="E4" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="F4" s="16">
+      <c r="F4" s="12">
         <v>12</v>
       </c>
       <c r="G4" s="2"/>
       <c r="H4" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="I4" s="14">
+      <c r="I4" s="10">
         <v>55.5</v>
       </c>
       <c r="J4" s="2"/>
@@ -1153,14 +1153,14 @@
       <c r="E5" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="F5" s="16">
+      <c r="F5" s="12">
         <v>21</v>
       </c>
       <c r="G5" s="2"/>
       <c r="H5" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="I5" s="15">
+      <c r="I5" s="11">
         <v>67.5</v>
       </c>
       <c r="J5" s="2"/>
@@ -1182,14 +1182,14 @@
       <c r="E6" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="F6" s="16">
+      <c r="F6" s="12">
         <v>27</v>
       </c>
       <c r="G6" s="2"/>
       <c r="H6" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="I6" s="17">
+      <c r="I6" s="13">
         <v>79.5</v>
       </c>
       <c r="J6" s="2"/>
@@ -1211,14 +1211,14 @@
       <c r="E7" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="F7" s="16">
+      <c r="F7" s="12">
         <v>33</v>
       </c>
       <c r="G7" s="2"/>
       <c r="H7" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="I7" s="18">
+      <c r="I7" s="14">
         <v>91.5</v>
       </c>
       <c r="J7" s="2"/>
@@ -1240,14 +1240,14 @@
       <c r="E8" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="F8" s="16">
+      <c r="F8" s="12">
         <v>39</v>
       </c>
       <c r="G8" s="2"/>
       <c r="H8" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="I8" s="19">
+      <c r="I8" s="15">
         <v>103.5</v>
       </c>
       <c r="J8" s="2"/>
@@ -1269,14 +1269,14 @@
       <c r="E9" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="F9" s="14">
+      <c r="F9" s="10">
         <v>45</v>
       </c>
       <c r="G9" s="2"/>
       <c r="H9" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="I9" s="20">
+      <c r="I9" s="16">
         <v>115.5</v>
       </c>
       <c r="J9" s="2"/>
@@ -1298,14 +1298,14 @@
       <c r="E10" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="F10" s="14">
+      <c r="F10" s="10">
         <v>51</v>
       </c>
       <c r="G10" s="2"/>
       <c r="H10" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="I10" s="21">
+      <c r="I10" s="17">
         <v>127.5</v>
       </c>
       <c r="J10" s="2"/>
@@ -1327,14 +1327,14 @@
       <c r="E11" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="F11" s="15">
+      <c r="F11" s="11">
         <v>57</v>
       </c>
       <c r="G11" s="2"/>
       <c r="H11" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="I11" s="22">
+      <c r="I11" s="18">
         <v>139.5</v>
       </c>
       <c r="J11" s="2"/>
@@ -1356,14 +1356,14 @@
       <c r="E12" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="F12" s="15">
+      <c r="F12" s="11">
         <v>63</v>
       </c>
       <c r="G12" s="2"/>
       <c r="H12" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="I12" s="23">
+      <c r="I12" s="19">
         <v>151.5</v>
       </c>
       <c r="J12" s="2"/>
@@ -1385,14 +1385,14 @@
       <c r="E13" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="F13" s="17">
+      <c r="F13" s="13">
         <v>69</v>
       </c>
       <c r="G13" s="2"/>
       <c r="H13" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="I13" s="24">
+      <c r="I13" s="20">
         <v>163.5</v>
       </c>
       <c r="J13" s="2"/>
@@ -1414,7 +1414,7 @@
       <c r="E14" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="F14" s="17">
+      <c r="F14" s="13">
         <v>72</v>
       </c>
       <c r="G14" s="2"/>
@@ -1443,7 +1443,7 @@
       <c r="E15" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="F15" s="17">
+      <c r="F15" s="13">
         <v>75</v>
       </c>
       <c r="G15" s="2"/>
@@ -1468,7 +1468,7 @@
       <c r="E16" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="F16" s="18">
+      <c r="F16" s="14">
         <v>78</v>
       </c>
       <c r="G16" s="2"/>
@@ -1493,7 +1493,7 @@
       <c r="E17" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="F17" s="18">
+      <c r="F17" s="14">
         <v>81</v>
       </c>
       <c r="G17" s="2"/>
@@ -1518,7 +1518,7 @@
       <c r="E18" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="F18" s="18">
+      <c r="F18" s="14">
         <v>84</v>
       </c>
       <c r="G18" s="2"/>
@@ -1543,7 +1543,7 @@
       <c r="E19" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="F19" s="18">
+      <c r="F19" s="14">
         <v>87</v>
       </c>
       <c r="G19" s="2"/>
@@ -1568,7 +1568,7 @@
       <c r="E20" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="F20" s="18">
+      <c r="F20" s="14">
         <v>90</v>
       </c>
       <c r="G20" s="2"/>
@@ -1593,7 +1593,7 @@
       <c r="E21" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="F21" s="19">
+      <c r="F21" s="15">
         <v>93</v>
       </c>
       <c r="G21" s="2"/>
@@ -1618,7 +1618,7 @@
       <c r="E22" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="F22" s="19">
+      <c r="F22" s="15">
         <v>96</v>
       </c>
       <c r="G22" s="2"/>
@@ -1643,7 +1643,7 @@
       <c r="E23" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="F23" s="19">
+      <c r="F23" s="15">
         <v>99</v>
       </c>
       <c r="G23" s="2"/>
@@ -1668,7 +1668,7 @@
       <c r="E24" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="F24" s="19">
+      <c r="F24" s="15">
         <v>102</v>
       </c>
       <c r="G24" s="2"/>
@@ -1693,7 +1693,7 @@
       <c r="E25" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="F25" s="20">
+      <c r="F25" s="16">
         <v>105</v>
       </c>
       <c r="G25" s="2"/>
@@ -1718,7 +1718,7 @@
       <c r="E26" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="F26" s="20">
+      <c r="F26" s="16">
         <v>108</v>
       </c>
       <c r="G26" s="2"/>
@@ -1743,7 +1743,7 @@
       <c r="E27" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="F27" s="20">
+      <c r="F27" s="16">
         <v>111</v>
       </c>
       <c r="G27" s="2"/>
@@ -1768,7 +1768,7 @@
       <c r="E28" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="F28" s="20">
+      <c r="F28" s="16">
         <v>114</v>
       </c>
       <c r="G28" s="2"/>
@@ -1793,7 +1793,7 @@
       <c r="E29" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="F29" s="21">
+      <c r="F29" s="17">
         <v>117</v>
       </c>
       <c r="G29" s="2"/>
@@ -1818,7 +1818,7 @@
       <c r="E30" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="F30" s="21">
+      <c r="F30" s="17">
         <v>120</v>
       </c>
       <c r="G30" s="2"/>
@@ -1843,7 +1843,7 @@
       <c r="E31" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="F31" s="21">
+      <c r="F31" s="17">
         <v>123</v>
       </c>
       <c r="G31" s="2"/>
@@ -1868,7 +1868,7 @@
       <c r="E32" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="F32" s="21">
+      <c r="F32" s="17">
         <v>126</v>
       </c>
       <c r="G32" s="2"/>
@@ -1893,7 +1893,7 @@
       <c r="E33" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="F33" s="22">
+      <c r="F33" s="18">
         <v>129</v>
       </c>
       <c r="G33" s="2"/>
@@ -1918,7 +1918,7 @@
       <c r="E34" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="F34" s="22">
+      <c r="F34" s="18">
         <v>132</v>
       </c>
       <c r="G34" s="2"/>
@@ -1943,7 +1943,7 @@
       <c r="E35" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="F35" s="22">
+      <c r="F35" s="18">
         <v>135</v>
       </c>
       <c r="G35" s="2"/>
@@ -1968,7 +1968,7 @@
       <c r="E36" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="F36" s="22">
+      <c r="F36" s="18">
         <v>138</v>
       </c>
       <c r="G36" s="2"/>
@@ -1993,7 +1993,7 @@
       <c r="E37" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="F37" s="23">
+      <c r="F37" s="19">
         <v>141</v>
       </c>
       <c r="G37" s="2"/>
@@ -2018,7 +2018,7 @@
       <c r="E38" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="F38" s="23">
+      <c r="F38" s="19">
         <v>144</v>
       </c>
       <c r="G38" s="2"/>
@@ -2043,7 +2043,7 @@
       <c r="E39" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="F39" s="23">
+      <c r="F39" s="19">
         <v>147</v>
       </c>
       <c r="G39" s="2"/>
@@ -2068,7 +2068,7 @@
       <c r="E40" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="F40" s="23">
+      <c r="F40" s="19">
         <v>150</v>
       </c>
       <c r="G40" s="2"/>
@@ -2093,8 +2093,8 @@
       <c r="E41" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="F41" s="24">
-        <v>156</v>
+      <c r="F41" s="20">
+        <v>20</v>
       </c>
       <c r="G41" s="2"/>
       <c r="H41" s="2"/>
@@ -2118,7 +2118,7 @@
       <c r="E42" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="F42" s="24">
+      <c r="F42" s="20">
         <v>162</v>
       </c>
       <c r="G42" s="2"/>

</xml_diff>